<commit_message>
Update schedule file: Y4_B2526_General_&_Special_Internal_1_B2_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_General_&_Special_Internal_1_B2_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_General_&_Special_Internal_1_B2_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2267,6 +2267,1406 @@
         <v>720</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>06/12/2025</t>
+        </is>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B53" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E53" s="7" t="inlineStr">
+        <is>
+          <t>07/12/2025</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G53" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B55" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C55" s="6" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E55" s="7" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G55" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B57" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C57" s="6" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E57" s="7" t="inlineStr">
+        <is>
+          <t>13/12/2025</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>14/12/2025</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B59" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E59" s="7" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G59" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E60" s="3" t="inlineStr">
+        <is>
+          <t>16/12/2025</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B61" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>cardiology</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E61" s="7" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G61" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B63" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C63" s="6" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D63" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E63" s="7" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G63" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="inlineStr">
+        <is>
+          <t>23/12/2025</t>
+        </is>
+      </c>
+      <c r="F64" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G64" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E65" s="7" t="inlineStr">
+        <is>
+          <t>24/12/2025</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E66" s="3" t="inlineStr">
+        <is>
+          <t>25/12/2025</t>
+        </is>
+      </c>
+      <c r="F66" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G66" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B67" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C67" s="6" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D67" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E67" s="7" t="inlineStr">
+        <is>
+          <t>28/12/2025</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G67" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+      <c r="F68" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C69" s="6" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E69" s="7" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G69" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E70" s="3" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="F70" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G70" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B71" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>chest</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E71" s="7" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G71" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>dermatology</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E72" s="3" t="inlineStr">
+        <is>
+          <t>04/01/2026</t>
+        </is>
+      </c>
+      <c r="F72" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B73" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>dermatology</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E73" s="7" t="inlineStr">
+        <is>
+          <t>05/01/2026</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G73" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>dermatology</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="inlineStr">
+        <is>
+          <t>06/01/2026</t>
+        </is>
+      </c>
+      <c r="F74" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G74" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>dermatology</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E75" s="7" t="inlineStr">
+        <is>
+          <t>07/01/2026</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
+          <t>dermatology</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="inlineStr">
+        <is>
+          <t>08/01/2026</t>
+        </is>
+      </c>
+      <c r="F76" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G76" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E77" s="7" t="inlineStr">
+        <is>
+          <t>23/11/2025</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G77" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E78" s="3" t="inlineStr">
+        <is>
+          <t>24/11/2025</t>
+        </is>
+      </c>
+      <c r="F78" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G78" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B79" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C79" s="6" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D79" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E79" s="7" t="inlineStr">
+        <is>
+          <t>25/11/2025</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G79" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="inlineStr">
+        <is>
+          <t>26/11/2025</t>
+        </is>
+      </c>
+      <c r="F80" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G80" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B81" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C81" s="6" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D81" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E81" s="7" t="inlineStr">
+        <is>
+          <t>27/11/2025</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E82" s="3" t="inlineStr">
+        <is>
+          <t>30/11/2025</t>
+        </is>
+      </c>
+      <c r="F82" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G82" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B83" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C83" s="6" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D83" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E83" s="7" t="inlineStr">
+        <is>
+          <t>01/12/2025</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E84" s="3" t="inlineStr">
+        <is>
+          <t>02/12/2025</t>
+        </is>
+      </c>
+      <c r="F84" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B85" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C85" s="6" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D85" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E85" s="7" t="inlineStr">
+        <is>
+          <t>03/12/2025</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>immunology/haematology</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E86" s="3" t="inlineStr">
+        <is>
+          <t>04/12/2025</t>
+        </is>
+      </c>
+      <c r="F86" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G86" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B87" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C87" s="6" t="inlineStr">
+        <is>
+          <t>tropical</t>
+        </is>
+      </c>
+      <c r="D87" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E87" s="7" t="inlineStr">
+        <is>
+          <t>11/01/2026</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>tropical</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E88" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026</t>
+        </is>
+      </c>
+      <c r="F88" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G88" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B89" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C89" s="6" t="inlineStr">
+        <is>
+          <t>tropical</t>
+        </is>
+      </c>
+      <c r="D89" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E89" s="7" t="inlineStr">
+        <is>
+          <t>13/01/2026</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>tropical</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E90" s="3" t="inlineStr">
+        <is>
+          <t>14/01/2026</t>
+        </is>
+      </c>
+      <c r="F90" s="4" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G90" s="5" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B91" s="6" t="inlineStr">
+        <is>
+          <t>INT-B2-B</t>
+        </is>
+      </c>
+      <c r="C91" s="6" t="inlineStr">
+        <is>
+          <t>tropical</t>
+        </is>
+      </c>
+      <c r="D91" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E91" s="7" t="inlineStr">
+        <is>
+          <t>15/01/2026</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>08:30:00</t>
+        </is>
+      </c>
+      <c r="G91" s="9" t="n">
+        <v>720</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upload Y4_B2526_General_&_Special_Internal_1_B2_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_General_&_Special_Internal_1_B2_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_General_&_Special_Internal_1_B2_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\modules_schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266A1B84-178E-4D2F-A9AD-76FCB9B749D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0627D1AC-B408-4F6B-A121-0A0DF05DB23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="580" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_&amp;_Special_Internal_1" sheetId="1" r:id="rId1"/>
@@ -739,7 +739,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -762,7 +762,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -785,7 +785,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -808,7 +808,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -831,7 +831,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -854,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -877,7 +877,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -900,7 +900,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -923,7 +923,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
       <c r="G11" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -969,7 +969,7 @@
         <v>12</v>
       </c>
       <c r="G12" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -992,7 +992,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1015,7 +1015,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1038,7 +1038,7 @@
         <v>12</v>
       </c>
       <c r="G15" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1061,7 +1061,7 @@
         <v>12</v>
       </c>
       <c r="G16" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1084,7 +1084,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1130,7 +1130,7 @@
         <v>12</v>
       </c>
       <c r="G19" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1153,7 +1153,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1176,7 +1176,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1199,7 +1199,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G22" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1222,7 +1222,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G23" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1245,7 +1245,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G24" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1268,7 +1268,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G25" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1291,7 +1291,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G26" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1314,7 +1314,7 @@
         <v>12</v>
       </c>
       <c r="G27" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1337,7 +1337,7 @@
         <v>12</v>
       </c>
       <c r="G28" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1360,7 +1360,7 @@
         <v>12</v>
       </c>
       <c r="G29" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1383,7 +1383,7 @@
         <v>12</v>
       </c>
       <c r="G30" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1406,7 +1406,7 @@
         <v>12</v>
       </c>
       <c r="G31" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1429,7 +1429,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G32" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1452,7 +1452,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G33" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1475,7 +1475,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G34" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1498,7 +1498,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G35" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1521,7 +1521,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G36" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1544,7 +1544,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G37" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1567,7 +1567,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G38" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1590,7 +1590,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G39" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1613,7 +1613,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G40" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1636,7 +1636,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G41" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1659,7 +1659,7 @@
         <v>12</v>
       </c>
       <c r="G42" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1682,7 +1682,7 @@
         <v>12</v>
       </c>
       <c r="G43" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1705,7 +1705,7 @@
         <v>12</v>
       </c>
       <c r="G44" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1728,7 +1728,7 @@
         <v>12</v>
       </c>
       <c r="G45" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1751,7 +1751,7 @@
         <v>12</v>
       </c>
       <c r="G46" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1774,7 +1774,7 @@
         <v>12</v>
       </c>
       <c r="G47" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1797,7 +1797,7 @@
         <v>12</v>
       </c>
       <c r="G48" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1820,7 +1820,7 @@
         <v>12</v>
       </c>
       <c r="G49" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -1843,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="G50" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -1866,7 +1866,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -1889,7 +1889,7 @@
         <v>12</v>
       </c>
       <c r="G52" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -1912,7 +1912,7 @@
         <v>12</v>
       </c>
       <c r="G53" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -1935,7 +1935,7 @@
         <v>12</v>
       </c>
       <c r="G54" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -1958,7 +1958,7 @@
         <v>12</v>
       </c>
       <c r="G55" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -1981,7 +1981,7 @@
         <v>12</v>
       </c>
       <c r="G56" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -2004,7 +2004,7 @@
         <v>12</v>
       </c>
       <c r="G57" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -2027,7 +2027,7 @@
         <v>12</v>
       </c>
       <c r="G58" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -2050,7 +2050,7 @@
         <v>12</v>
       </c>
       <c r="G59" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -2073,7 +2073,7 @@
         <v>12</v>
       </c>
       <c r="G60" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -2096,7 +2096,7 @@
         <v>12</v>
       </c>
       <c r="G61" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -2119,7 +2119,7 @@
         <v>12</v>
       </c>
       <c r="G62" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2142,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="G63" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -2165,7 +2165,7 @@
         <v>12</v>
       </c>
       <c r="G64" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -2188,7 +2188,7 @@
         <v>12</v>
       </c>
       <c r="G65" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2211,7 +2211,7 @@
         <v>12</v>
       </c>
       <c r="G66" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2234,7 +2234,7 @@
         <v>12</v>
       </c>
       <c r="G67" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2257,7 +2257,7 @@
         <v>12</v>
       </c>
       <c r="G68" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -2280,7 +2280,7 @@
         <v>12</v>
       </c>
       <c r="G69" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -2303,7 +2303,7 @@
         <v>12</v>
       </c>
       <c r="G70" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -2326,7 +2326,7 @@
         <v>12</v>
       </c>
       <c r="G71" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -2349,7 +2349,7 @@
         <v>12</v>
       </c>
       <c r="G72" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -2372,7 +2372,7 @@
         <v>12</v>
       </c>
       <c r="G73" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2395,7 +2395,7 @@
         <v>12</v>
       </c>
       <c r="G74" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -2418,7 +2418,7 @@
         <v>12</v>
       </c>
       <c r="G75" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -2441,7 +2441,7 @@
         <v>12</v>
       </c>
       <c r="G76" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -2464,7 +2464,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G77" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -2487,7 +2487,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G78" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -2510,7 +2510,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G79" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -2533,7 +2533,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G80" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -2556,7 +2556,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G81" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -2579,7 +2579,7 @@
         <v>12</v>
       </c>
       <c r="G82" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -2602,7 +2602,7 @@
         <v>12</v>
       </c>
       <c r="G83" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -2625,7 +2625,7 @@
         <v>12</v>
       </c>
       <c r="G84" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -2648,7 +2648,7 @@
         <v>12</v>
       </c>
       <c r="G85" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -2671,7 +2671,7 @@
         <v>12</v>
       </c>
       <c r="G86" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -2694,7 +2694,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G87" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -2717,7 +2717,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G88" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -2740,7 +2740,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G89" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -2763,7 +2763,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G90" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -2786,7 +2786,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G91" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -2809,7 +2809,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G92" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -2832,7 +2832,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G93" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
@@ -2855,7 +2855,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G94" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -2878,7 +2878,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G95" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
@@ -2901,7 +2901,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G96" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
@@ -2924,7 +2924,7 @@
         <v>12</v>
       </c>
       <c r="G97" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
@@ -2947,7 +2947,7 @@
         <v>12</v>
       </c>
       <c r="G98" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
@@ -2970,7 +2970,7 @@
         <v>12</v>
       </c>
       <c r="G99" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
@@ -2993,7 +2993,7 @@
         <v>12</v>
       </c>
       <c r="G100" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
@@ -3016,7 +3016,7 @@
         <v>12</v>
       </c>
       <c r="G101" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
@@ -3039,7 +3039,7 @@
         <v>12</v>
       </c>
       <c r="G102" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
@@ -3062,7 +3062,7 @@
         <v>12</v>
       </c>
       <c r="G103" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
@@ -3085,7 +3085,7 @@
         <v>12</v>
       </c>
       <c r="G104" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
@@ -3108,7 +3108,7 @@
         <v>12</v>
       </c>
       <c r="G105" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
@@ -3131,7 +3131,7 @@
         <v>12</v>
       </c>
       <c r="G106" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
@@ -3154,7 +3154,7 @@
         <v>12</v>
       </c>
       <c r="G107" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
@@ -3177,7 +3177,7 @@
         <v>12</v>
       </c>
       <c r="G108" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
@@ -3200,7 +3200,7 @@
         <v>12</v>
       </c>
       <c r="G109" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
@@ -3223,7 +3223,7 @@
         <v>12</v>
       </c>
       <c r="G110" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
@@ -3246,7 +3246,7 @@
         <v>12</v>
       </c>
       <c r="G111" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
@@ -3269,7 +3269,7 @@
         <v>12</v>
       </c>
       <c r="G112" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
@@ -3292,7 +3292,7 @@
         <v>12</v>
       </c>
       <c r="G113" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
@@ -3315,7 +3315,7 @@
         <v>12</v>
       </c>
       <c r="G114" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
@@ -3338,7 +3338,7 @@
         <v>12</v>
       </c>
       <c r="G115" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
@@ -3361,7 +3361,7 @@
         <v>12</v>
       </c>
       <c r="G116" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
@@ -3384,7 +3384,7 @@
         <v>12</v>
       </c>
       <c r="G117" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
@@ -3407,7 +3407,7 @@
         <v>12</v>
       </c>
       <c r="G118" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
@@ -3430,7 +3430,7 @@
         <v>12</v>
       </c>
       <c r="G119" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
@@ -3453,7 +3453,7 @@
         <v>12</v>
       </c>
       <c r="G120" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
@@ -3476,7 +3476,7 @@
         <v>12</v>
       </c>
       <c r="G121" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -3499,7 +3499,7 @@
         <v>12</v>
       </c>
       <c r="G122" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -3522,7 +3522,7 @@
         <v>12</v>
       </c>
       <c r="G123" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
@@ -3545,7 +3545,7 @@
         <v>12</v>
       </c>
       <c r="G124" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
@@ -3568,7 +3568,7 @@
         <v>12</v>
       </c>
       <c r="G125" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -3591,7 +3591,7 @@
         <v>12</v>
       </c>
       <c r="G126" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -3614,7 +3614,7 @@
         <v>12</v>
       </c>
       <c r="G127" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
@@ -3637,7 +3637,7 @@
         <v>12</v>
       </c>
       <c r="G128" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
@@ -3660,7 +3660,7 @@
         <v>12</v>
       </c>
       <c r="G129" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
@@ -3683,7 +3683,7 @@
         <v>12</v>
       </c>
       <c r="G130" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
@@ -3706,7 +3706,7 @@
         <v>12</v>
       </c>
       <c r="G131" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
@@ -3729,7 +3729,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G132" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
@@ -3752,7 +3752,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G133" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
@@ -3775,7 +3775,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G134" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
@@ -3798,7 +3798,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G135" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
@@ -3821,7 +3821,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G136" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
@@ -3844,7 +3844,7 @@
         <v>12</v>
       </c>
       <c r="G137" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
@@ -3867,7 +3867,7 @@
         <v>12</v>
       </c>
       <c r="G138" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
@@ -3890,7 +3890,7 @@
         <v>12</v>
       </c>
       <c r="G139" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
@@ -3913,7 +3913,7 @@
         <v>12</v>
       </c>
       <c r="G140" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
@@ -3936,7 +3936,7 @@
         <v>12</v>
       </c>
       <c r="G141" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
@@ -3959,7 +3959,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G142" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
@@ -3982,7 +3982,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G143" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
@@ -4005,7 +4005,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G144" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
@@ -4028,7 +4028,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G145" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
@@ -4051,7 +4051,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G146" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
@@ -4074,7 +4074,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G147" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
@@ -4097,7 +4097,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G148" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
@@ -4120,7 +4120,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G149" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
@@ -4143,7 +4143,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G150" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
@@ -4166,7 +4166,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G151" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
@@ -4189,7 +4189,7 @@
         <v>12</v>
       </c>
       <c r="G152" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
@@ -4212,7 +4212,7 @@
         <v>12</v>
       </c>
       <c r="G153" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
@@ -4235,7 +4235,7 @@
         <v>12</v>
       </c>
       <c r="G154" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
@@ -4258,7 +4258,7 @@
         <v>12</v>
       </c>
       <c r="G155" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
@@ -4281,7 +4281,7 @@
         <v>12</v>
       </c>
       <c r="G156" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
@@ -4304,7 +4304,7 @@
         <v>12</v>
       </c>
       <c r="G157" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
@@ -4327,7 +4327,7 @@
         <v>12</v>
       </c>
       <c r="G158" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
@@ -4350,7 +4350,7 @@
         <v>12</v>
       </c>
       <c r="G159" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
@@ -4373,7 +4373,7 @@
         <v>12</v>
       </c>
       <c r="G160" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
@@ -4396,7 +4396,7 @@
         <v>12</v>
       </c>
       <c r="G161" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
@@ -4419,7 +4419,7 @@
         <v>12</v>
       </c>
       <c r="G162" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
@@ -4442,7 +4442,7 @@
         <v>12</v>
       </c>
       <c r="G163" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
@@ -4465,7 +4465,7 @@
         <v>12</v>
       </c>
       <c r="G164" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
@@ -4488,7 +4488,7 @@
         <v>12</v>
       </c>
       <c r="G165" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
@@ -4511,7 +4511,7 @@
         <v>12</v>
       </c>
       <c r="G166" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
@@ -4534,7 +4534,7 @@
         <v>12</v>
       </c>
       <c r="G167" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
@@ -4557,7 +4557,7 @@
         <v>12</v>
       </c>
       <c r="G168" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
@@ -4580,7 +4580,7 @@
         <v>12</v>
       </c>
       <c r="G169" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
@@ -4603,7 +4603,7 @@
         <v>12</v>
       </c>
       <c r="G170" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
@@ -4626,7 +4626,7 @@
         <v>12</v>
       </c>
       <c r="G171" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.35">
@@ -4649,7 +4649,7 @@
         <v>12</v>
       </c>
       <c r="G172" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
@@ -4672,7 +4672,7 @@
         <v>12</v>
       </c>
       <c r="G173" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
@@ -4695,7 +4695,7 @@
         <v>12</v>
       </c>
       <c r="G174" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.35">
@@ -4718,7 +4718,7 @@
         <v>12</v>
       </c>
       <c r="G175" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
@@ -4741,7 +4741,7 @@
         <v>12</v>
       </c>
       <c r="G176" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.35">
@@ -4764,7 +4764,7 @@
         <v>12</v>
       </c>
       <c r="G177" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.35">
@@ -4787,7 +4787,7 @@
         <v>12</v>
       </c>
       <c r="G178" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
@@ -4810,7 +4810,7 @@
         <v>12</v>
       </c>
       <c r="G179" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.35">
@@ -4833,7 +4833,7 @@
         <v>12</v>
       </c>
       <c r="G180" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.35">
@@ -4856,7 +4856,7 @@
         <v>12</v>
       </c>
       <c r="G181" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.35">
@@ -4879,7 +4879,7 @@
         <v>12</v>
       </c>
       <c r="G182" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
@@ -4902,7 +4902,7 @@
         <v>12</v>
       </c>
       <c r="G183" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.35">
@@ -4925,7 +4925,7 @@
         <v>12</v>
       </c>
       <c r="G184" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.35">
@@ -4948,7 +4948,7 @@
         <v>12</v>
       </c>
       <c r="G185" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.35">
@@ -4971,7 +4971,7 @@
         <v>12</v>
       </c>
       <c r="G186" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.35">
@@ -4994,7 +4994,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G187" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.35">
@@ -5017,7 +5017,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G188" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.35">
@@ -5040,7 +5040,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G189" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.35">
@@ -5063,7 +5063,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G190" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.35">
@@ -5086,7 +5086,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G191" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.35">
@@ -5109,7 +5109,7 @@
         <v>12</v>
       </c>
       <c r="G192" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.35">
@@ -5132,7 +5132,7 @@
         <v>12</v>
       </c>
       <c r="G193" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
@@ -5155,7 +5155,7 @@
         <v>12</v>
       </c>
       <c r="G194" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.35">
@@ -5178,7 +5178,7 @@
         <v>12</v>
       </c>
       <c r="G195" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.35">
@@ -5201,7 +5201,7 @@
         <v>12</v>
       </c>
       <c r="G196" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.35">
@@ -5224,7 +5224,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G197" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.35">
@@ -5247,7 +5247,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G198" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.35">
@@ -5270,7 +5270,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G199" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.35">
@@ -5293,7 +5293,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G200" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.35">
@@ -5316,7 +5316,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G201" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.35">
@@ -5339,7 +5339,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G202" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.35">
@@ -5362,7 +5362,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G203" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.35">
@@ -5385,7 +5385,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G204" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.35">
@@ -5408,7 +5408,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G205" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.35">
@@ -5431,7 +5431,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G206" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.35">
@@ -5454,7 +5454,7 @@
         <v>12</v>
       </c>
       <c r="G207" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.35">
@@ -5477,7 +5477,7 @@
         <v>12</v>
       </c>
       <c r="G208" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.35">
@@ -5500,7 +5500,7 @@
         <v>12</v>
       </c>
       <c r="G209" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.35">
@@ -5523,7 +5523,7 @@
         <v>12</v>
       </c>
       <c r="G210" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.35">
@@ -5546,7 +5546,7 @@
         <v>12</v>
       </c>
       <c r="G211" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.35">
@@ -5569,7 +5569,7 @@
         <v>12</v>
       </c>
       <c r="G212" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.35">
@@ -5592,7 +5592,7 @@
         <v>12</v>
       </c>
       <c r="G213" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.35">
@@ -5615,7 +5615,7 @@
         <v>12</v>
       </c>
       <c r="G214" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.35">
@@ -5638,7 +5638,7 @@
         <v>12</v>
       </c>
       <c r="G215" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.35">
@@ -5661,7 +5661,7 @@
         <v>12</v>
       </c>
       <c r="G216" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.35">
@@ -5684,7 +5684,7 @@
         <v>12</v>
       </c>
       <c r="G217" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.35">
@@ -5707,7 +5707,7 @@
         <v>12</v>
       </c>
       <c r="G218" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.35">
@@ -5730,7 +5730,7 @@
         <v>12</v>
       </c>
       <c r="G219" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.35">
@@ -5753,7 +5753,7 @@
         <v>12</v>
       </c>
       <c r="G220" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.35">
@@ -5776,7 +5776,7 @@
         <v>12</v>
       </c>
       <c r="G221" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.35">
@@ -5799,7 +5799,7 @@
         <v>12</v>
       </c>
       <c r="G222" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.35">
@@ -5822,7 +5822,7 @@
         <v>12</v>
       </c>
       <c r="G223" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.35">
@@ -5845,7 +5845,7 @@
         <v>12</v>
       </c>
       <c r="G224" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.35">
@@ -5868,7 +5868,7 @@
         <v>12</v>
       </c>
       <c r="G225" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.35">
@@ -5891,7 +5891,7 @@
         <v>12</v>
       </c>
       <c r="G226" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.35">
@@ -5914,7 +5914,7 @@
         <v>12</v>
       </c>
       <c r="G227" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.35">
@@ -5937,7 +5937,7 @@
         <v>12</v>
       </c>
       <c r="G228" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.35">
@@ -5960,7 +5960,7 @@
         <v>12</v>
       </c>
       <c r="G229" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.35">
@@ -5983,7 +5983,7 @@
         <v>12</v>
       </c>
       <c r="G230" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.35">
@@ -6006,7 +6006,7 @@
         <v>12</v>
       </c>
       <c r="G231" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.35">
@@ -6029,7 +6029,7 @@
         <v>12</v>
       </c>
       <c r="G232" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.35">
@@ -6052,7 +6052,7 @@
         <v>12</v>
       </c>
       <c r="G233" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.35">
@@ -6075,7 +6075,7 @@
         <v>12</v>
       </c>
       <c r="G234" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.35">
@@ -6098,7 +6098,7 @@
         <v>12</v>
       </c>
       <c r="G235" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.35">
@@ -6121,7 +6121,7 @@
         <v>12</v>
       </c>
       <c r="G236" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.35">
@@ -6144,7 +6144,7 @@
         <v>12</v>
       </c>
       <c r="G237" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.35">
@@ -6167,7 +6167,7 @@
         <v>12</v>
       </c>
       <c r="G238" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.35">
@@ -6190,7 +6190,7 @@
         <v>12</v>
       </c>
       <c r="G239" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.35">
@@ -6213,7 +6213,7 @@
         <v>12</v>
       </c>
       <c r="G240" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.35">
@@ -6236,7 +6236,7 @@
         <v>12</v>
       </c>
       <c r="G241" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.35">
@@ -6259,7 +6259,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G242" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.35">
@@ -6282,7 +6282,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G243" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.35">
@@ -6305,7 +6305,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G244" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
@@ -6328,7 +6328,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G245" s="9">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.35">
@@ -6351,7 +6351,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G246" s="5">
-        <v>180</v>
+        <v>900</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.35">
@@ -6374,7 +6374,7 @@
         <v>12</v>
       </c>
       <c r="G247" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.35">
@@ -6397,7 +6397,7 @@
         <v>12</v>
       </c>
       <c r="G248" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.35">
@@ -6420,7 +6420,7 @@
         <v>12</v>
       </c>
       <c r="G249" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.35">
@@ -6443,7 +6443,7 @@
         <v>12</v>
       </c>
       <c r="G250" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.35">
@@ -6466,7 +6466,7 @@
         <v>12</v>
       </c>
       <c r="G251" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.35">
@@ -6489,7 +6489,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G252" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.35">
@@ -6512,7 +6512,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G253" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.35">
@@ -6535,7 +6535,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G254" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.35">
@@ -6558,7 +6558,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G255" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.35">
@@ -6581,7 +6581,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G256" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.35">
@@ -6604,7 +6604,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G257" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.35">
@@ -6627,7 +6627,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G258" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.35">
@@ -6650,7 +6650,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G259" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.35">
@@ -6673,7 +6673,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G260" s="5">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.35">
@@ -6696,7 +6696,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="G261" s="9">
-        <v>240</v>
+        <v>900</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.35">
@@ -6719,7 +6719,7 @@
         <v>12</v>
       </c>
       <c r="G262" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.35">
@@ -6742,7 +6742,7 @@
         <v>12</v>
       </c>
       <c r="G263" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.35">
@@ -6765,7 +6765,7 @@
         <v>12</v>
       </c>
       <c r="G264" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.35">
@@ -6788,7 +6788,7 @@
         <v>12</v>
       </c>
       <c r="G265" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.35">
@@ -6811,7 +6811,7 @@
         <v>12</v>
       </c>
       <c r="G266" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.35">
@@ -6834,7 +6834,7 @@
         <v>12</v>
       </c>
       <c r="G267" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.35">
@@ -6857,7 +6857,7 @@
         <v>12</v>
       </c>
       <c r="G268" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.35">
@@ -6880,7 +6880,7 @@
         <v>12</v>
       </c>
       <c r="G269" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.35">
@@ -6903,7 +6903,7 @@
         <v>12</v>
       </c>
       <c r="G270" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.35">
@@ -6926,7 +6926,7 @@
         <v>12</v>
       </c>
       <c r="G271" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.35">
@@ -6949,7 +6949,7 @@
         <v>12</v>
       </c>
       <c r="G272" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.35">
@@ -6972,7 +6972,7 @@
         <v>12</v>
       </c>
       <c r="G273" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.35">
@@ -6995,7 +6995,7 @@
         <v>12</v>
       </c>
       <c r="G274" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.35">
@@ -7018,7 +7018,7 @@
         <v>12</v>
       </c>
       <c r="G275" s="9">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.35">
@@ -7041,7 +7041,7 @@
         <v>12</v>
       </c>
       <c r="G276" s="5">
-        <v>360</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>